<commit_message>
added write up & other missing files
</commit_message>
<xml_diff>
--- a/Resources/City Geo Join Table.xlsx
+++ b/Resources/City Geo Join Table.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremykalmus/Desktop/Google Drive/UC Davis Analytics Boot Camp/Projects/project_one/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BAE245-807B-CA47-A11F-EBA7BAB06FEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A00B43-D1D9-E94B-9635-5FC8B6BE39C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="9860" windowWidth="28040" windowHeight="17440" xr2:uid="{99D83BBD-EFF5-1C4C-B23A-92DC18DA2657}"/>
+    <workbookView xWindow="7900" yWindow="9860" windowWidth="28040" windowHeight="17440" xr2:uid="{99D83BBD-EFF5-1C4C-B23A-92DC18DA2657}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>City</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Tampa, FL</t>
+  </si>
+  <si>
+    <t>City, State</t>
   </si>
 </sst>
 </file>
@@ -643,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B361E1F-B667-454A-8076-94A3E8E554B3}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,348 +658,519 @@
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="str">
+        <f>LEFT(A2, SEARCH(",",A2,1)-1)</f>
+        <v>Albany</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C43" si="0">LEFT(A3, SEARCH(",",A3,1)-1)</f>
+        <v>Atlanta</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>Baltimore</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>Boise</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>Boston</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>Buffalo</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>Charlotte</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>Chicago</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>Cincinnati</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>Columbus</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>Dallas</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>Denver</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>Detroit</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>Grand Rapids</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>Harrisburg</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>Hartford</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Houston</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Indianapolis</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Jacksonville</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Las Vegas</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>Los Angeles</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>Louisville</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Miami</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Nashville</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>New Orleans</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>Orlando</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>Philadelphia</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>Phoenix</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>Pittsburgh</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>Portland</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>Raleigh</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>Richmond</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>Roanoke</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B37" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>San Diego</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>San Francisco</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>Seattle</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>Spokane</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>St. Louis</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>Syracuse</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>Tampa</v>
       </c>
     </row>
   </sheetData>

</xml_diff>